<commit_message>
Added description to tasks
</commit_message>
<xml_diff>
--- a/Battleship/doc/scrum/scrum.xlsx
+++ b/Battleship/doc/scrum/scrum.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23812"/>
-  <workbookPr autoCompressPictures="0"/>
+  <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="341" activeTab="1"/>
   </bookViews>
@@ -13,6 +13,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sprint Backlog'!$A$1:$J$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Sprint Backlog'!$A$1:$F$12</definedName>
   </definedNames>
   <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -120,13 +121,49 @@
   </si>
   <si>
     <t>Krenger</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>Implementation des Kommunikationsaufbaus und Erkennung des Gegenspielers über das Netzwerk</t>
+  </si>
+  <si>
+    <t>Implementation der Netzwerkkommunikation für die Durchführung des Spiels</t>
+  </si>
+  <si>
+    <t>Erstellung eines groben Designs für das Spiel (Start-Bildschirm, Spielbildschirm, …)</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>Logik</t>
+  </si>
+  <si>
+    <t>Erstellung der UI-Komponenten für Java</t>
+  </si>
+  <si>
+    <t>Zusammenfügen der Komponenten zu einem Programm (GUI)</t>
+  </si>
+  <si>
+    <t>Definition der Schnittstellen zu den Modulen Netzwerkkommunikation und GUI</t>
+  </si>
+  <si>
+    <t>Implementation der Schnittstellen</t>
+  </si>
+  <si>
+    <t>Implementation der Grundklassen für das Spiel</t>
+  </si>
+  <si>
+    <t>Implementation der Spiellogik</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -154,6 +191,12 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -786,15 +829,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection sqref="A1:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="3" max="3" width="35.1640625" customWidth="1"/>
     <col min="4" max="4" width="23.83203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.1640625" bestFit="1" customWidth="1"/>
@@ -836,7 +882,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="8">
         <v>1</v>
       </c>
       <c r="C2" t="s">
@@ -856,7 +902,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="8">
         <v>1</v>
       </c>
       <c r="C3" t="s">
@@ -865,53 +911,74 @@
       <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
       <c r="F3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" ht="56">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="8">
         <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
       <c r="F4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" ht="42">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="8">
         <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
       <c r="F5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" ht="56">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="8">
         <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
       <c r="F6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" ht="28">
       <c r="A7">
         <v>6</v>
       </c>
@@ -921,52 +988,91 @@
       <c r="C7" t="s">
         <v>24</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
       <c r="F7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" ht="42">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="8">
         <v>3</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
       </c>
+      <c r="D8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
       <c r="F8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" ht="56">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" s="8">
+        <v>1</v>
+      </c>
       <c r="C9" t="s">
         <v>28</v>
       </c>
+      <c r="D9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
       <c r="F9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="13.25" customHeight="1">
+    <row r="10" spans="1:10" ht="28">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="C10" t="s">
         <v>27</v>
       </c>
+      <c r="D10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
       <c r="F10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" ht="28">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="C11" t="s">
         <v>29</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
       </c>
       <c r="F11" t="s">
         <v>31</v>
@@ -976,23 +1082,49 @@
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" s="8">
+        <v>3</v>
+      </c>
       <c r="C12" t="s">
         <v>30</v>
       </c>
+      <c r="D12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
       <c r="F12" t="s">
         <v>31</v>
       </c>
     </row>
+    <row r="13" spans="1:10">
+      <c r="B13" s="8"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" s="8"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="B15" s="8"/>
+    </row>
     <row r="16" spans="1:10">
+      <c r="B16" s="8"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="5:5">
+    <row r="17" spans="2:5">
+      <c r="B17" s="8"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="31" spans="5:5">
+    <row r="18" spans="2:5">
+      <c r="B18" s="8"/>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="8"/>
+    </row>
+    <row r="31" spans="2:5">
       <c r="E31" s="6"/>
     </row>
-    <row r="32" spans="5:5">
+    <row r="32" spans="2:5">
       <c r="E32" s="6"/>
     </row>
     <row r="33" spans="1:5">
@@ -1005,11 +1137,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:J36"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="80" firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>

<commit_message>
Added coordinates to Missile, added comments and TODOs
</commit_message>
<xml_diff>
--- a/Battleship/doc/scrum/scrum.xlsx
+++ b/Battleship/doc/scrum/scrum.xlsx
@@ -835,14 +835,14 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection sqref="A1:F12"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="35.1640625" customWidth="1"/>
     <col min="4" max="4" width="23.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -897,6 +897,12 @@
       <c r="F2" t="s">
         <v>18</v>
       </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="42">
       <c r="A3">
@@ -917,6 +923,12 @@
       <c r="F3" t="s">
         <v>18</v>
       </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:10" ht="56">
       <c r="A4">
@@ -937,6 +949,9 @@
       <c r="F4" t="s">
         <v>18</v>
       </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:10" ht="42">
       <c r="A5">
@@ -957,6 +972,9 @@
       <c r="F5" t="s">
         <v>18</v>
       </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:10" ht="56">
       <c r="A6">
@@ -977,6 +995,9 @@
       <c r="F6" t="s">
         <v>12</v>
       </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="28">
       <c r="A7">
@@ -997,6 +1018,9 @@
       <c r="F7" t="s">
         <v>12</v>
       </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:10" ht="42">
       <c r="A8">
@@ -1017,6 +1041,9 @@
       <c r="F8" t="s">
         <v>12</v>
       </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:10" ht="56">
       <c r="A9">
@@ -1037,6 +1064,9 @@
       <c r="F9" t="s">
         <v>31</v>
       </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:10" ht="28">
       <c r="A10">
@@ -1057,6 +1087,9 @@
       <c r="F10" t="s">
         <v>31</v>
       </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="28">
       <c r="A11">
@@ -1077,6 +1110,9 @@
       <c r="F11" t="s">
         <v>31</v>
       </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12">
@@ -1096,6 +1132,9 @@
       </c>
       <c r="F12" t="s">
         <v>31</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10">

</xml_diff>